<commit_message>
Updated HCW Upload Excel
</commit_message>
<xml_diff>
--- a/public/reg.xlsx
+++ b/public/reg.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22904"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6528BE7-24AA-4BC1-A679-386DA7CA60DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4D6AC0BC-5248-450D-BAC2-B800D5F663D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -169,8 +169,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A1:A5"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -500,6 +501,7 @@
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
     <col min="6" max="6" width="26.42578125" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -531,18 +533,21 @@
         <v>8</v>
       </c>
     </row>
+    <row r="2" spans="1:9">
+      <c r="H2" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="textLength" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{A0A2CBAF-CE91-46DB-A50F-208563A83425}">
+    <dataValidation type="textLength" errorStyle="warning" operator="greaterThan" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="This field is required" sqref="A1:A1048576" xr:uid="{A0A2CBAF-CE91-46DB-A50F-208563A83425}">
       <formula1>3</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{9364F8CB-AB5B-4694-9FE7-D61DEDB4BFEA}">
+    <dataValidation type="textLength" errorStyle="warning" operator="greaterThan" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="This field is required" sqref="B1:B1048576" xr:uid="{9364F8CB-AB5B-4694-9FE7-D61DEDB4BFEA}">
       <formula1>2</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{D0AED352-5A8F-4875-ABED-EBF63D0EB8B5}">
+    <dataValidation type="whole" errorStyle="warning" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="This field is required" sqref="C1:C1048576" xr:uid="{D0AED352-5A8F-4875-ABED-EBF63D0EB8B5}">
       <formula1>9</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{B10CC5CF-87A6-43F1-9440-552069FB56D2}">
+    <dataValidation type="date" operator="lessThanOrEqual" showInputMessage="1" showErrorMessage="1" errorTitle="Date Format" error="Insert date using dd/mm/yyyy eg 01/01/2002" sqref="H1:H1048576" xr:uid="{B10CC5CF-87A6-43F1-9440-552069FB56D2}">
       <formula1>37257</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>